<commit_message>
* Some tiny updates
</commit_message>
<xml_diff>
--- a/static/data/cards.xlsx
+++ b/static/data/cards.xlsx
@@ -592,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,6 +863,7 @@
       <c r="J12" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="K12" s="6"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
@@ -886,6 +887,7 @@
       <c r="J13" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="K13" s="6"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
@@ -909,6 +911,7 @@
       <c r="J14" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="K14" s="6"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
@@ -934,6 +937,7 @@
       <c r="J15" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="K15" s="6"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
@@ -959,8 +963,9 @@
       <c r="J16" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K16" s="6"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
         <v>15</v>
       </c>
@@ -984,8 +989,9 @@
       <c r="J17" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K17" s="6"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
         <v>16</v>
       </c>
@@ -1007,8 +1013,9 @@
       <c r="J18" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K18" s="6"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
         <v>17</v>
       </c>
@@ -1030,18 +1037,19 @@
       <c r="J19" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K19" s="6"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
         <v>20</v>
       </c>
@@ -1065,8 +1073,9 @@
       <c r="J22" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K22" s="6"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
         <v>21</v>
       </c>
@@ -1090,8 +1099,9 @@
       <c r="J23" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K23" s="6"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
         <v>22</v>
       </c>
@@ -1115,8 +1125,9 @@
       <c r="J24" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K24" s="6"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
         <v>23</v>
       </c>
@@ -1140,8 +1151,9 @@
       <c r="J25" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K25" s="6"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
         <v>24</v>
       </c>
@@ -1163,8 +1175,9 @@
       <c r="J26" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K26" s="6"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="2">
         <v>25</v>
       </c>
@@ -1186,8 +1199,9 @@
       <c r="J27" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K27" s="6"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
         <v>26</v>
       </c>
@@ -1195,7 +1209,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="2">
         <v>27</v>
       </c>
@@ -1218,7 +1232,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="2">
         <v>28</v>
       </c>
@@ -1241,7 +1255,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="2">
         <v>29</v>
       </c>
@@ -1264,12 +1278,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" s="2">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="2">
         <v>31</v>
       </c>
@@ -1293,8 +1307,9 @@
       <c r="J33" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K33" s="6"/>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" s="2">
         <v>32</v>
       </c>
@@ -1318,8 +1333,9 @@
       <c r="J34" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K34" s="6"/>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" s="2">
         <v>33</v>
       </c>
@@ -1343,8 +1359,9 @@
       <c r="J35" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K35" s="6"/>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" s="2">
         <v>34</v>
       </c>
@@ -1372,33 +1389,34 @@
       <c r="J36" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K36" s="6"/>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37" s="2">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38" s="2">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" s="2">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" s="2">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" s="2">
         <v>40</v>
       </c>

</xml_diff>